<commit_message>
update app to moduals
</commit_message>
<xml_diff>
--- a/Sarah_data/Data_S1.xlsx
+++ b/Sarah_data/Data_S1.xlsx
@@ -1,72 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Github_Projects\Brenner_Graphs\Sarah_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig.1A" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Fig.1B" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Fig.1C" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Fig.2A" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Fig.2B" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Fig.2C" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Fig.1A" sheetId="1" r:id="rId1"/>
+    <sheet name="Fig.1B" sheetId="2" r:id="rId2"/>
+    <sheet name="Fig.1C" sheetId="3" r:id="rId3"/>
+    <sheet name="Fig.2A" sheetId="4" r:id="rId4"/>
+    <sheet name="Fig.2B" sheetId="5" r:id="rId5"/>
+    <sheet name="Fig.2C" sheetId="6" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t xml:space="preserve">Sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Man2afl/fl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD25 (MFI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">αCD3/28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Man2afl/flCD4cre+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD69 (MFI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD44 (MFI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p-S6 (MFI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p-mTOR (MFI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD98 (MFI)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="24">
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>Man2afl/fl</t>
+  </si>
+  <si>
+    <t>CD25 (MFI)</t>
+  </si>
+  <si>
+    <t>αCD3/28</t>
+  </si>
+  <si>
+    <t>Man2afl/flCD4cre+</t>
+  </si>
+  <si>
+    <t>Sw</t>
+  </si>
+  <si>
+    <t>CD69 (MFI)</t>
+  </si>
+  <si>
+    <t>CD44 (MFI)</t>
+  </si>
+  <si>
+    <t>p-S6 (MFI)</t>
+  </si>
+  <si>
+    <t>p-mTOR (MFI)</t>
+  </si>
+  <si>
+    <t>CD98 (MFI)</t>
+  </si>
+  <si>
+    <t>Unit_Log</t>
+  </si>
+  <si>
+    <t>Annotation_1</t>
+  </si>
+  <si>
+    <t>Annotation_label_1</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Annotation_label_2</t>
+  </si>
+  <si>
+    <t>Annotation_2</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>0h</t>
+  </si>
+  <si>
+    <t>6h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,13 +131,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -383,14 +429,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="A2:D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,11 +452,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>7226</v>
       </c>
       <c r="C2" t="s">
@@ -418,11 +466,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>9881</v>
       </c>
       <c r="C3" t="s">
@@ -432,11 +480,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>11570</v>
       </c>
       <c r="C4" t="s">
@@ -446,11 +494,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>10180</v>
       </c>
       <c r="C5" t="s">
@@ -460,11 +508,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>6882</v>
       </c>
       <c r="C6" t="s">
@@ -474,11 +522,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>7575</v>
       </c>
       <c r="C7" t="s">
@@ -488,11 +536,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>12252</v>
       </c>
       <c r="C8" t="s">
@@ -502,11 +550,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>8906</v>
       </c>
       <c r="C9" t="s">
@@ -516,11 +564,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>7624</v>
       </c>
       <c r="C10" t="s">
@@ -530,11 +578,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>9806</v>
       </c>
       <c r="C11" t="s">
@@ -544,11 +592,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>10724</v>
       </c>
       <c r="C12" t="s">
@@ -558,11 +606,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>9586</v>
       </c>
       <c r="C13" t="s">
@@ -572,11 +620,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>6574</v>
       </c>
       <c r="C14" t="s">
@@ -586,11 +634,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>7267</v>
       </c>
       <c r="C15" t="s">
@@ -600,11 +648,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>12260</v>
       </c>
       <c r="C16" t="s">
@@ -614,11 +662,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>8841</v>
       </c>
       <c r="C17" t="s">
@@ -630,19 +678,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,11 +704,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>8596</v>
       </c>
       <c r="C2" t="s">
@@ -670,11 +718,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>9924</v>
       </c>
       <c r="C3" t="s">
@@ -684,11 +732,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>10731</v>
       </c>
       <c r="C4" t="s">
@@ -698,11 +746,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>10597</v>
       </c>
       <c r="C5" t="s">
@@ -712,11 +760,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>8923</v>
       </c>
       <c r="C6" t="s">
@@ -726,11 +774,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>10615</v>
       </c>
       <c r="C7" t="s">
@@ -740,11 +788,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>12147</v>
       </c>
       <c r="C8" t="s">
@@ -754,11 +802,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>11632</v>
       </c>
       <c r="C9" t="s">
@@ -768,11 +816,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>14552</v>
       </c>
       <c r="C10" t="s">
@@ -782,11 +830,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>16159</v>
       </c>
       <c r="C11" t="s">
@@ -796,11 +844,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>16757</v>
       </c>
       <c r="C12" t="s">
@@ -810,11 +858,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>17231</v>
       </c>
       <c r="C13" t="s">
@@ -824,11 +872,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>14695</v>
       </c>
       <c r="C14" t="s">
@@ -838,11 +886,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>14703</v>
       </c>
       <c r="C15" t="s">
@@ -852,11 +900,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>17789</v>
       </c>
       <c r="C16" t="s">
@@ -866,11 +914,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>15641</v>
       </c>
       <c r="C17" t="s">
@@ -882,19 +930,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,11 +956,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>22871</v>
       </c>
       <c r="C2" t="s">
@@ -922,11 +970,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>23057</v>
       </c>
       <c r="C3" t="s">
@@ -936,11 +984,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>28720</v>
       </c>
       <c r="C4" t="s">
@@ -950,11 +998,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>29376</v>
       </c>
       <c r="C5" t="s">
@@ -964,11 +1012,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>21274</v>
       </c>
       <c r="C6" t="s">
@@ -978,11 +1026,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>23542</v>
       </c>
       <c r="C7" t="s">
@@ -992,11 +1040,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>40958</v>
       </c>
       <c r="C8" t="s">
@@ -1006,11 +1054,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>33566</v>
       </c>
       <c r="C9" t="s">
@@ -1020,11 +1068,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>24544</v>
       </c>
       <c r="C10" t="s">
@@ -1034,11 +1082,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>25197</v>
       </c>
       <c r="C11" t="s">
@@ -1048,11 +1096,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>28239</v>
       </c>
       <c r="C12" t="s">
@@ -1062,11 +1110,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>32108</v>
       </c>
       <c r="C13" t="s">
@@ -1076,11 +1124,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>22575</v>
       </c>
       <c r="C14" t="s">
@@ -1090,11 +1138,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>25130</v>
       </c>
       <c r="C15" t="s">
@@ -1104,11 +1152,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>41212</v>
       </c>
       <c r="C16" t="s">
@@ -1118,11 +1166,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>35830</v>
       </c>
       <c r="C17" t="s">
@@ -1134,19 +1182,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,11 +1208,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>7844</v>
       </c>
       <c r="C2" t="s">
@@ -1174,11 +1222,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>8247</v>
       </c>
       <c r="C3" t="s">
@@ -1188,11 +1236,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>8986</v>
       </c>
       <c r="C4" t="s">
@@ -1202,11 +1250,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>9838</v>
       </c>
       <c r="C5" t="s">
@@ -1216,11 +1264,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>6718</v>
       </c>
       <c r="C6" t="s">
@@ -1230,11 +1278,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>7270</v>
       </c>
       <c r="C7" t="s">
@@ -1244,11 +1292,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>8500</v>
       </c>
       <c r="C8" t="s">
@@ -1258,11 +1306,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>6720</v>
       </c>
       <c r="C9" t="s">
@@ -1272,11 +1320,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>7812</v>
       </c>
       <c r="C10" t="s">
@@ -1286,11 +1334,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>6902</v>
       </c>
       <c r="C11" t="s">
@@ -1300,11 +1348,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>8835</v>
       </c>
       <c r="C12" t="s">
@@ -1314,11 +1362,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>7448</v>
       </c>
       <c r="C13" t="s">
@@ -1328,11 +1376,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>5910</v>
       </c>
       <c r="C14" t="s">
@@ -1342,11 +1390,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>6711</v>
       </c>
       <c r="C15" t="s">
@@ -1356,11 +1404,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>7979</v>
       </c>
       <c r="C16" t="s">
@@ -1370,11 +1418,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>6434</v>
       </c>
       <c r="C17" t="s">
@@ -1386,19 +1434,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1412,11 +1460,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1679</v>
       </c>
       <c r="C2" t="s">
@@ -1426,11 +1474,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1798</v>
       </c>
       <c r="C3" t="s">
@@ -1440,11 +1488,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>1735</v>
       </c>
       <c r="C4" t="s">
@@ -1454,11 +1502,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>1458</v>
       </c>
       <c r="C5" t="s">
@@ -1468,11 +1516,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>1082</v>
       </c>
       <c r="C6" t="s">
@@ -1482,11 +1530,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>955</v>
       </c>
       <c r="C7" t="s">
@@ -1496,11 +1544,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>1203</v>
       </c>
       <c r="C8" t="s">
@@ -1510,11 +1558,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>1035</v>
       </c>
       <c r="C9" t="s">
@@ -1524,11 +1572,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>1349</v>
       </c>
       <c r="C10" t="s">
@@ -1538,11 +1586,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>1306</v>
       </c>
       <c r="C11" t="s">
@@ -1552,11 +1600,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>1270</v>
       </c>
       <c r="C12" t="s">
@@ -1566,11 +1614,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1148</v>
       </c>
       <c r="C13" t="s">
@@ -1580,11 +1628,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>946</v>
       </c>
       <c r="C14" t="s">
@@ -1594,11 +1642,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>802</v>
       </c>
       <c r="C15" t="s">
@@ -1608,11 +1656,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>1153</v>
       </c>
       <c r="C16" t="s">
@@ -1622,11 +1670,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>907</v>
       </c>
       <c r="C17" t="s">
@@ -1638,19 +1686,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1658,238 +1708,232 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2445</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>2749</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>2765</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>2656</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>2042</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1807</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>2909</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>2557</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>4391</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>5097</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>5725</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>5330</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>4212</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>4565</v>
       </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>5360</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>4617</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>